<commit_message>
added a couple things
</commit_message>
<xml_diff>
--- a/Compiled_synchrony_experiment_data.xlsx
+++ b/Compiled_synchrony_experiment_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/justinbenjamin/Desktop/McMaster/Synchrony/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{3E75E0B1-0F42-174A-86C4-C303BE39D051}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{67481920-3293-AB46-8F97-B7F16EFF0C75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="13620" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="13420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hatch_success_by_chick" sheetId="1" r:id="rId1"/>
@@ -18,9 +18,9 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hatch_success_by_chick!$A$1:$AB$275</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sheet1!$A$1:$AJ$43</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sheet1!$A$1:$AJ$44</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="1412" uniqueCount="184">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="1416" uniqueCount="185">
   <si>
     <t>Nest</t>
   </si>
@@ -593,6 +593,9 @@
   </si>
   <si>
     <t xml:space="preserve">NH4,NB3,NB2,NH2,NB1,NH1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">No swaps at all </t>
   </si>
 </sst>
 </file>
@@ -11711,11 +11714,12 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1169386B-F813-034E-AA1A-A149472682C8}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:AJ145"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:XFD1048576"/>
+      <selection pane="bottomLeft" activeCell="K49" sqref="K49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11947,7 +11951,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A4" s="10">
         <v>2018</v>
       </c>
@@ -12081,8 +12085,11 @@
       <c r="V5" s="10">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="W5" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A6" s="10">
         <v>2018</v>
       </c>
@@ -12151,7 +12158,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A7" s="10">
         <v>2018</v>
       </c>
@@ -12217,7 +12224,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A8" s="10">
         <v>2018</v>
       </c>
@@ -12286,7 +12293,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A9" s="10">
         <v>2018</v>
       </c>
@@ -12417,6 +12424,9 @@
       <c r="V10" s="10">
         <v>3</v>
       </c>
+      <c r="W10" t="s">
+        <v>184</v>
+      </c>
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A11" s="10">
@@ -12483,8 +12493,11 @@
       <c r="V11" s="10">
         <v>3</v>
       </c>
-    </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="W11" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A12" s="10">
         <v>2018</v>
       </c>
@@ -12615,8 +12628,11 @@
       <c r="V13" s="10">
         <v>2</v>
       </c>
-    </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="W13" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A14" s="10">
         <v>2018</v>
       </c>
@@ -12754,7 +12770,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A16" s="10">
         <v>2018</v>
       </c>
@@ -12823,7 +12839,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="17" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:33" hidden="1" x14ac:dyDescent="0.2">
       <c r="A17" s="10">
         <v>2018</v>
       </c>
@@ -12889,7 +12905,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:33" hidden="1" x14ac:dyDescent="0.2">
       <c r="A18" s="10">
         <v>2018</v>
       </c>
@@ -12955,7 +12971,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:33" hidden="1" x14ac:dyDescent="0.2">
       <c r="A19" s="10">
         <v>2018</v>
       </c>
@@ -13021,7 +13037,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:33" hidden="1" x14ac:dyDescent="0.2">
       <c r="A20" s="10">
         <v>2018</v>
       </c>
@@ -13085,7 +13101,7 @@
       </c>
       <c r="V20" s="10"/>
     </row>
-    <row r="21" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:33" hidden="1" x14ac:dyDescent="0.2">
       <c r="A21" s="10">
         <v>2018</v>
       </c>
@@ -13151,7 +13167,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:33" hidden="1" x14ac:dyDescent="0.2">
       <c r="A22" s="10">
         <v>2018</v>
       </c>
@@ -13286,7 +13302,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:33" hidden="1" x14ac:dyDescent="0.2">
       <c r="A24" s="10">
         <v>2018</v>
       </c>
@@ -13352,7 +13368,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:33" hidden="1" x14ac:dyDescent="0.2">
       <c r="A25" s="10">
         <v>2018</v>
       </c>
@@ -13418,7 +13434,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:33" hidden="1" x14ac:dyDescent="0.2">
       <c r="A26" s="10">
         <v>2023</v>
       </c>
@@ -13489,7 +13505,7 @@
       <c r="AD26" s="4"/>
       <c r="AG26" s="3"/>
     </row>
-    <row r="27" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:33" hidden="1" x14ac:dyDescent="0.2">
       <c r="A27" s="10">
         <v>2023</v>
       </c>
@@ -13560,7 +13576,7 @@
       <c r="AD27" s="4"/>
       <c r="AG27" s="3"/>
     </row>
-    <row r="28" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:33" hidden="1" x14ac:dyDescent="0.2">
       <c r="A28" s="10">
         <v>2023</v>
       </c>
@@ -13699,7 +13715,7 @@
       <c r="AC29" s="4"/>
       <c r="AG29" s="3"/>
     </row>
-    <row r="30" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:33" hidden="1" x14ac:dyDescent="0.2">
       <c r="A30" s="10">
         <v>2023</v>
       </c>
@@ -13769,7 +13785,7 @@
       <c r="AC30" s="4"/>
       <c r="AG30" s="3"/>
     </row>
-    <row r="31" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:33" hidden="1" x14ac:dyDescent="0.2">
       <c r="A31" s="10">
         <v>2023</v>
       </c>
@@ -13909,7 +13925,7 @@
       <c r="AC32" s="4"/>
       <c r="AG32" s="3"/>
     </row>
-    <row r="33" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:36" hidden="1" x14ac:dyDescent="0.2">
       <c r="A33" s="10">
         <v>2023</v>
       </c>
@@ -13978,7 +13994,7 @@
       </c>
       <c r="AG33" s="3"/>
     </row>
-    <row r="34" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:36" hidden="1" x14ac:dyDescent="0.2">
       <c r="A34" s="10">
         <v>2023</v>
       </c>
@@ -14116,7 +14132,7 @@
       </c>
       <c r="AG35" s="3"/>
     </row>
-    <row r="36" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:36" hidden="1" x14ac:dyDescent="0.2">
       <c r="A36" s="10">
         <v>2023</v>
       </c>
@@ -14188,7 +14204,7 @@
       <c r="AG36" s="3"/>
       <c r="AJ36" s="4"/>
     </row>
-    <row r="37" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:36" hidden="1" x14ac:dyDescent="0.2">
       <c r="A37" s="10">
         <v>2023</v>
       </c>
@@ -14257,7 +14273,7 @@
       </c>
       <c r="AG37" s="3"/>
     </row>
-    <row r="38" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:36" hidden="1" x14ac:dyDescent="0.2">
       <c r="A38" s="10">
         <v>2023</v>
       </c>
@@ -14326,7 +14342,7 @@
       </c>
       <c r="AG38" s="3"/>
     </row>
-    <row r="39" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:36" hidden="1" x14ac:dyDescent="0.2">
       <c r="A39" s="14">
         <v>2024</v>
       </c>
@@ -14395,7 +14411,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="40" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:36" hidden="1" x14ac:dyDescent="0.2">
       <c r="A40" s="14">
         <v>2024</v>
       </c>
@@ -14463,7 +14479,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="41" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:36" hidden="1" x14ac:dyDescent="0.2">
       <c r="A41" s="14">
         <v>2024</v>
       </c>
@@ -14527,7 +14543,7 @@
       </c>
       <c r="V41" s="10"/>
     </row>
-    <row r="42" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:36" hidden="1" x14ac:dyDescent="0.2">
       <c r="A42" s="14">
         <v>2024</v>
       </c>
@@ -14595,7 +14611,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:36" hidden="1" x14ac:dyDescent="0.2">
       <c r="A43" s="14">
         <v>2024</v>
       </c>
@@ -14663,7 +14679,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:36" hidden="1" x14ac:dyDescent="0.2">
       <c r="A44" s="14">
         <v>2024</v>
       </c>
@@ -15123,7 +15139,13 @@
       <c r="B145" s="3"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AJ43" xr:uid="{1169386B-F813-034E-AA1A-A149472682C8}"/>
+  <autoFilter ref="A1:AJ44" xr:uid="{1169386B-F813-034E-AA1A-A149472682C8}">
+    <filterColumn colId="14">
+      <filters>
+        <filter val="0"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fixed survival column name
</commit_message>
<xml_diff>
--- a/Compiled_synchrony_experiment_data.xlsx
+++ b/Compiled_synchrony_experiment_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/justinbenjamin/Desktop/McMaster/Synchrony/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{DAE6A200-6DFD-414A-A376-F9B5E7F7717B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{C0F5CB93-419D-FE4D-9A7C-D0BF3E75C8A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="13380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -143,9 +143,6 @@
     <t>M16 East</t>
   </si>
   <si>
-    <t>Surival_60</t>
-  </si>
-  <si>
     <t>Location</t>
   </si>
   <si>
@@ -567,6 +564,9 @@
   </si>
   <si>
     <t>Estimated_hatch_spread</t>
+  </si>
+  <si>
+    <t>Survival_60</t>
   </si>
 </sst>
 </file>
@@ -1472,9 +1472,9 @@
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1169386B-F813-034E-AA1A-A149472682C8}">
   <dimension ref="A1:AK145"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E12" sqref="E12"/>
+      <selection pane="bottomLeft" activeCell="W1" sqref="W1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1502,70 +1502,70 @@
         <v>24</v>
       </c>
       <c r="B1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C1" s="8" t="s">
         <v>0</v>
       </c>
       <c r="D1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E1" t="s">
         <v>25</v>
       </c>
       <c r="F1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G1" t="s">
         <v>1</v>
       </c>
       <c r="H1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="I1" t="s">
+        <v>98</v>
+      </c>
+      <c r="J1" t="s">
         <v>99</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
+        <v>135</v>
+      </c>
+      <c r="L1" t="s">
+        <v>166</v>
+      </c>
+      <c r="M1" t="s">
+        <v>97</v>
+      </c>
+      <c r="N1" t="s">
         <v>100</v>
       </c>
-      <c r="K1" t="s">
-        <v>136</v>
-      </c>
-      <c r="L1" t="s">
-        <v>167</v>
-      </c>
-      <c r="M1" t="s">
-        <v>98</v>
-      </c>
-      <c r="N1" t="s">
-        <v>101</v>
-      </c>
       <c r="O1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="P1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="Q1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="R1" t="s">
+        <v>80</v>
+      </c>
+      <c r="S1" t="s">
         <v>81</v>
       </c>
-      <c r="S1" t="s">
-        <v>82</v>
-      </c>
       <c r="T1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="U1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="V1" t="s">
         <v>2</v>
       </c>
       <c r="W1" t="s">
-        <v>34</v>
+        <v>175</v>
       </c>
       <c r="X1" t="s">
         <v>26</v>
@@ -1576,10 +1576,10 @@
         <v>2018</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D2" s="3" t="d">
         <v>2018-08-22</v>
@@ -1589,7 +1589,7 @@
         <v>7</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H2" s="6" t="d">
         <v>2018-09-03</v>
@@ -1598,16 +1598,16 @@
         <v>2018-09-07</v>
       </c>
       <c r="J2" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="L2" s="13" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="M2" s="11" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="N2" s="12">
         <v>1</v>
@@ -1622,16 +1622,16 @@
         <v>6</v>
       </c>
       <c r="R2" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="S2" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="T2" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="U2" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="V2" s="8">
         <v>0</v>
@@ -1640,7 +1640,7 @@
         <v>0</v>
       </c>
       <c r="X2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.2">
@@ -1648,10 +1648,10 @@
         <v>2018</v>
       </c>
       <c r="B3" s="17" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D3" s="3" t="d">
         <v>2018-08-18</v>
@@ -1661,25 +1661,25 @@
         <v>5</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="H3" s="6" t="d">
         <v>2018-09-03</v>
       </c>
       <c r="I3" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J3" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K3" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="L3" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="M3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="N3" s="12">
         <v>1</v>
@@ -1694,16 +1694,16 @@
         <v>0</v>
       </c>
       <c r="R3" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="S3" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="T3" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="U3" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="V3" s="8">
         <v>0</v>
@@ -1712,7 +1712,7 @@
         <v>0</v>
       </c>
       <c r="X3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.2">
@@ -1720,7 +1720,7 @@
         <v>2018</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C4" s="8" t="s">
         <v>3</v>
@@ -1733,25 +1733,25 @@
         <v>10</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H4" s="6" t="d">
         <v>2018-09-13</v>
       </c>
       <c r="I4" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J4" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K4" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="L4" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="M4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="N4" s="12">
         <v>1</v>
@@ -1784,7 +1784,7 @@
         <v>3</v>
       </c>
       <c r="X4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.2">
@@ -1792,7 +1792,7 @@
         <v>2018</v>
       </c>
       <c r="B5" s="17" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C5" s="8" t="s">
         <v>8</v>
@@ -1805,7 +1805,7 @@
         <v>9</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H5" s="6" t="d">
         <v>2018-09-17</v>
@@ -1814,16 +1814,16 @@
         <v>2018-09-30</v>
       </c>
       <c r="J5" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K5" t="s">
+        <v>142</v>
+      </c>
+      <c r="L5" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="M5" s="16" t="s">
         <v>143</v>
-      </c>
-      <c r="L5" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="M5" s="16" t="s">
-        <v>144</v>
       </c>
       <c r="N5" s="8">
         <v>2</v>
@@ -1856,7 +1856,7 @@
         <v>2</v>
       </c>
       <c r="X5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.2">
@@ -1864,10 +1864,10 @@
         <v>2018</v>
       </c>
       <c r="B6" s="17" t="s">
+        <v>156</v>
+      </c>
+      <c r="C6" s="8" t="s">
         <v>157</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>158</v>
       </c>
       <c r="D6" s="3" t="d">
         <v>2018-09-15</v>
@@ -1877,25 +1877,25 @@
         <v>9</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H6" s="6" t="d">
         <v>2018-09-17</v>
       </c>
       <c r="I6" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J6" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K6" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="L6" s="13" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="M6" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="N6" s="12">
         <v>1</v>
@@ -1910,16 +1910,16 @@
         <v>9</v>
       </c>
       <c r="R6" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="S6" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="T6" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="U6" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="V6" s="8">
         <v>0</v>
@@ -1933,7 +1933,7 @@
         <v>2018</v>
       </c>
       <c r="B7" s="17" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C7" s="8" t="s">
         <v>9</v>
@@ -1946,25 +1946,25 @@
         <v>7</v>
       </c>
       <c r="G7" s="8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H7" s="6" t="d">
         <v>2018-09-17</v>
       </c>
       <c r="I7" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J7" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K7" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="L7" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="M7" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="N7" s="12">
         <v>1</v>
@@ -1997,7 +1997,7 @@
         <v>3</v>
       </c>
       <c r="X7" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.2">
@@ -2005,10 +2005,10 @@
         <v>2018</v>
       </c>
       <c r="B8" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D8" s="3" t="d">
         <v>2018-09-12</v>
@@ -2018,25 +2018,25 @@
         <v>5</v>
       </c>
       <c r="G8" s="8" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="H8" s="6" t="d">
         <v>2018-09-17</v>
       </c>
       <c r="I8" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J8" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K8" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="L8" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="M8" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="N8" s="12">
         <v>1</v>
@@ -2051,16 +2051,16 @@
         <v>5</v>
       </c>
       <c r="R8" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="S8" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="T8" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="U8" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="V8" s="8">
         <v>0</v>
@@ -2074,7 +2074,7 @@
         <v>2018</v>
       </c>
       <c r="B9" s="17" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C9" s="8" t="s">
         <v>12</v>
@@ -2087,25 +2087,25 @@
         <v>7</v>
       </c>
       <c r="G9" s="8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H9" s="6" t="d">
         <v>2018-09-01</v>
       </c>
       <c r="I9" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J9" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K9" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="L9" s="13" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="M9" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="N9" s="12">
         <v>1</v>
@@ -2143,7 +2143,7 @@
         <v>2018</v>
       </c>
       <c r="B10" s="17" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C10" s="8" t="s">
         <v>14</v>
@@ -2156,25 +2156,25 @@
         <v>5</v>
       </c>
       <c r="G10" s="8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H10" s="6" t="d">
         <v>2018-09-01</v>
       </c>
       <c r="I10" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J10" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K10" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="L10" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="M10" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="N10" s="12">
         <v>1</v>
@@ -2207,7 +2207,7 @@
         <v>3</v>
       </c>
       <c r="X10" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="11" spans="1:24" x14ac:dyDescent="0.2">
@@ -2215,7 +2215,7 @@
         <v>2018</v>
       </c>
       <c r="B11" s="17" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C11" s="8" t="s">
         <v>15</v>
@@ -2228,7 +2228,7 @@
         <v>7</v>
       </c>
       <c r="G11" s="8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H11" s="6" t="d">
         <v>2018-08-30</v>
@@ -2237,16 +2237,16 @@
         <v>2018-09-01</v>
       </c>
       <c r="J11" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K11" s="15" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="L11" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="M11" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="N11" s="8">
         <v>2</v>
@@ -2279,7 +2279,7 @@
         <v>2</v>
       </c>
       <c r="X11" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="12" spans="1:24" x14ac:dyDescent="0.2">
@@ -2287,7 +2287,7 @@
         <v>2018</v>
       </c>
       <c r="B12" s="17" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C12" s="8" t="s">
         <v>16</v>
@@ -2300,25 +2300,25 @@
         <v>8</v>
       </c>
       <c r="G12" s="8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H12" s="6" t="d">
         <v>2018-08-28</v>
       </c>
       <c r="I12" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J12" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K12" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="L12" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="M12" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="N12" s="12">
         <v>1</v>
@@ -2351,7 +2351,7 @@
         <v>2</v>
       </c>
       <c r="X12" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="13" spans="1:24" x14ac:dyDescent="0.2">
@@ -2359,7 +2359,7 @@
         <v>2018</v>
       </c>
       <c r="B13" s="17" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C13" s="8" t="s">
         <v>17</v>
@@ -2372,7 +2372,7 @@
         <v>10</v>
       </c>
       <c r="G13" s="8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H13" s="6" t="d">
         <v>2018-09-13</v>
@@ -2381,16 +2381,16 @@
         <v>2018-09-17</v>
       </c>
       <c r="J13" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K13" t="s">
+        <v>139</v>
+      </c>
+      <c r="L13" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="M13" t="s">
         <v>140</v>
-      </c>
-      <c r="L13" s="13" t="s">
-        <v>83</v>
-      </c>
-      <c r="M13" t="s">
-        <v>141</v>
       </c>
       <c r="N13" s="8">
         <v>2</v>
@@ -2428,7 +2428,7 @@
         <v>2018</v>
       </c>
       <c r="B14" s="17" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C14" s="8" t="s">
         <v>6</v>
@@ -2441,25 +2441,25 @@
         <v>8</v>
       </c>
       <c r="G14" s="8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H14" s="6" t="d">
         <v>2018-09-17</v>
       </c>
       <c r="I14" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J14" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K14" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="L14" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="M14" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="N14" s="12">
         <v>1</v>
@@ -2497,7 +2497,7 @@
         <v>2018</v>
       </c>
       <c r="B15" s="17" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C15" s="8" t="s">
         <v>18</v>
@@ -2510,25 +2510,25 @@
         <v>8</v>
       </c>
       <c r="G15" s="8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H15" s="6" t="d">
         <v>2018-09-17</v>
       </c>
       <c r="I15" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J15" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K15" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="L15" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="M15" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="N15" s="12">
         <v>1</v>
@@ -2566,10 +2566,10 @@
         <v>2018</v>
       </c>
       <c r="B16" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D16" s="3" t="d">
         <v>2018-09-17</v>
@@ -2579,7 +2579,7 @@
         <v>6</v>
       </c>
       <c r="G16" s="8" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="H16" s="6" t="d">
         <v>2018-09-22</v>
@@ -2588,16 +2588,16 @@
         <v>2018-09-27</v>
       </c>
       <c r="J16" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K16" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="L16" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="M16" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="N16" s="12">
         <v>2</v>
@@ -2633,7 +2633,7 @@
         <v>2018</v>
       </c>
       <c r="B17" s="17" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C17" s="8" t="s">
         <v>19</v>
@@ -2646,7 +2646,7 @@
         <v>7</v>
       </c>
       <c r="G17" s="8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H17" s="6" t="d">
         <v>2018-09-22</v>
@@ -2655,16 +2655,16 @@
         <v>2018-09-25</v>
       </c>
       <c r="J17" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K17" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="L17" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="M17" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="N17" s="8">
         <v>2</v>
@@ -2702,7 +2702,7 @@
         <v>2018</v>
       </c>
       <c r="B18" s="17" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C18" s="8" t="s">
         <v>20</v>
@@ -2715,25 +2715,25 @@
         <v>12</v>
       </c>
       <c r="G18" s="8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H18" s="6" t="d">
         <v>2018-09-27</v>
       </c>
       <c r="I18" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J18" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K18" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="L18" s="13" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="M18" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="N18" s="12">
         <v>1</v>
@@ -2766,7 +2766,7 @@
         <v>0</v>
       </c>
       <c r="X18" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="19" spans="1:34" x14ac:dyDescent="0.2">
@@ -2774,7 +2774,7 @@
         <v>2018</v>
       </c>
       <c r="B19" s="17" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C19" s="8" t="s">
         <v>21</v>
@@ -2787,7 +2787,7 @@
         <v>6</v>
       </c>
       <c r="G19" s="8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H19" s="6" t="d">
         <v>2018-09-15</v>
@@ -2796,16 +2796,16 @@
         <v>2018-09-17</v>
       </c>
       <c r="J19" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K19" s="15" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L19" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="M19" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="N19" s="8">
         <v>2</v>
@@ -2843,7 +2843,7 @@
         <v>2018</v>
       </c>
       <c r="B20" s="17" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C20" s="8" t="s">
         <v>22</v>
@@ -2856,25 +2856,25 @@
         <v>7</v>
       </c>
       <c r="G20" s="8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H20" s="6" t="d">
         <v>2018-09-22</v>
       </c>
       <c r="I20" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J20" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K20" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="L20" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="M20" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="N20" s="8">
         <v>1</v>
@@ -2912,7 +2912,7 @@
         <v>2018</v>
       </c>
       <c r="B21" s="17" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C21" s="8" t="s">
         <v>23</v>
@@ -2925,7 +2925,7 @@
         <v>7</v>
       </c>
       <c r="G21" s="8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H21" s="6" t="d">
         <v>2018-09-19</v>
@@ -2937,13 +2937,13 @@
         <v>2018-09-30</v>
       </c>
       <c r="K21" t="s">
+        <v>169</v>
+      </c>
+      <c r="L21" t="s">
         <v>170</v>
       </c>
-      <c r="L21" t="s">
-        <v>171</v>
-      </c>
       <c r="M21" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="N21" s="12">
         <v>3</v>
@@ -2981,7 +2981,7 @@
         <v>2018</v>
       </c>
       <c r="B22" s="17" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C22" s="8" t="s">
         <v>10</v>
@@ -2994,25 +2994,25 @@
         <v>8</v>
       </c>
       <c r="G22" s="8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H22" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I22" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J22" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K22" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="L22" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="M22" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="N22" s="12">
         <v>0</v>
@@ -3045,7 +3045,7 @@
         <v>3</v>
       </c>
       <c r="X22" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="Z22" s="8"/>
     </row>
@@ -3054,7 +3054,7 @@
         <v>2018</v>
       </c>
       <c r="B23" s="17" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C23" s="8" t="s">
         <v>11</v>
@@ -3067,25 +3067,25 @@
         <v>6</v>
       </c>
       <c r="G23" s="8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H23" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I23" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J23" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K23" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="L23" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="M23" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="N23" s="12">
         <v>0</v>
@@ -3118,7 +3118,7 @@
         <v>4</v>
       </c>
       <c r="X23" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="Z23" s="8"/>
     </row>
@@ -3127,7 +3127,7 @@
         <v>2018</v>
       </c>
       <c r="B24" s="17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C24" s="8" t="s">
         <v>7</v>
@@ -3140,25 +3140,25 @@
         <v>7</v>
       </c>
       <c r="G24" s="8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H24" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I24" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J24" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K24" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="L24" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="M24" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="N24" s="8">
         <v>0</v>
@@ -3191,7 +3191,7 @@
         <v>3</v>
       </c>
       <c r="X24" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="Z24" s="8"/>
     </row>
@@ -3200,7 +3200,7 @@
         <v>2018</v>
       </c>
       <c r="B25" s="17" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C25" s="8" t="s">
         <v>13</v>
@@ -3213,25 +3213,25 @@
         <v>7</v>
       </c>
       <c r="G25" s="8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H25" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I25" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J25" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K25" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="L25" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="M25" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="N25" s="12">
         <v>0</v>
@@ -3264,7 +3264,7 @@
         <v>2</v>
       </c>
       <c r="X25" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="Z25" s="8"/>
     </row>
@@ -3273,7 +3273,7 @@
         <v>2023</v>
       </c>
       <c r="B26" s="15" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C26" s="8" t="s">
         <v>5</v>
@@ -3288,25 +3288,25 @@
         <v>8</v>
       </c>
       <c r="G26" s="8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H26" s="6" t="d">
         <v>2023-09-04</v>
       </c>
       <c r="I26" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J26" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K26" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="L26" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="M26" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="N26" s="12">
         <v>1</v>
@@ -3347,7 +3347,7 @@
         <v>2023</v>
       </c>
       <c r="B27" s="15" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C27" s="8" t="s">
         <v>15</v>
@@ -3362,25 +3362,25 @@
         <v>8</v>
       </c>
       <c r="G27" s="8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H27" s="6" t="d">
         <v>2023-09-04</v>
       </c>
       <c r="I27" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J27" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K27" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="L27" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="M27" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="N27" s="12">
         <v>1</v>
@@ -3421,10 +3421,10 @@
         <v>2023</v>
       </c>
       <c r="B28" s="15" t="s">
+        <v>150</v>
+      </c>
+      <c r="C28" s="8" t="s">
         <v>151</v>
-      </c>
-      <c r="C28" s="8" t="s">
-        <v>152</v>
       </c>
       <c r="D28" s="5" t="d">
         <v>2023-08-20</v>
@@ -3434,25 +3434,25 @@
         <v>5</v>
       </c>
       <c r="G28" s="8" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="H28" s="6" t="d">
         <v>2023-09-04</v>
       </c>
       <c r="I28" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J28" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K28" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="L28" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="M28" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="N28" s="12">
         <v>1</v>
@@ -3473,7 +3473,7 @@
         <v>2023-09-13</v>
       </c>
       <c r="T28" s="10" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="U28" s="14">
         <v>3</v>
@@ -3493,10 +3493,10 @@
         <v>2023</v>
       </c>
       <c r="B29" s="15" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D29" s="5" t="d">
         <v>2023-08-20</v>
@@ -3514,19 +3514,19 @@
         <v>2023-09-04</v>
       </c>
       <c r="I29" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J29" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K29" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="L29" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="M29" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="N29" s="12">
         <v>1</v>
@@ -3547,7 +3547,7 @@
         <v>2023-09-14</v>
       </c>
       <c r="T29" s="10" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="U29" s="8">
         <v>11</v>
@@ -3566,10 +3566,10 @@
         <v>2023</v>
       </c>
       <c r="B30" s="15" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D30" s="5" t="d">
         <v>2023-09-01</v>
@@ -3581,25 +3581,25 @@
         <v>12</v>
       </c>
       <c r="G30" s="8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H30" s="6" t="d">
         <v>2023-09-15</v>
       </c>
       <c r="I30" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J30" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K30" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="L30" s="13" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="M30" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="N30" s="12">
         <v>1</v>
@@ -3639,7 +3639,7 @@
         <v>2023</v>
       </c>
       <c r="B31" s="15" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C31" s="8" t="s">
         <v>11</v>
@@ -3654,25 +3654,25 @@
         <v>9</v>
       </c>
       <c r="G31" s="8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H31" s="6" t="d">
         <v>2023-09-15</v>
       </c>
       <c r="I31" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J31" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K31" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="L31" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="M31" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="N31" s="12">
         <v>1</v>
@@ -3712,7 +3712,7 @@
         <v>2023</v>
       </c>
       <c r="B32" s="15" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C32" s="8" t="s">
         <v>21</v>
@@ -3733,19 +3733,19 @@
         <v>2023-09-15</v>
       </c>
       <c r="I32" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J32" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K32" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="L32" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="M32" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="N32" s="12">
         <v>1</v>
@@ -3766,7 +3766,7 @@
         <v>2023-10-04</v>
       </c>
       <c r="T32" s="7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="U32" s="8">
         <v>4</v>
@@ -3785,10 +3785,10 @@
         <v>2023</v>
       </c>
       <c r="B33" s="15" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C33" s="8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D33" s="5" t="d">
         <v>2023-09-29</v>
@@ -3800,25 +3800,25 @@
         <v>8</v>
       </c>
       <c r="G33" s="8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H33" s="6" t="d">
         <v>2023-10-07</v>
       </c>
       <c r="I33" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J33" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K33" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="L33" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="M33" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="N33" s="12">
         <v>1</v>
@@ -3857,40 +3857,40 @@
         <v>2023</v>
       </c>
       <c r="B34" s="15" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C34" s="8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D34" s="5" t="d">
         <v>2023-10-05</v>
       </c>
       <c r="E34" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F34" s="8">
         <v>8</v>
       </c>
       <c r="G34" s="8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H34" s="6" t="d">
         <v>2023-10-07</v>
       </c>
       <c r="I34" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J34" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K34" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="L34" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="M34" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="N34" s="12">
         <v>1</v>
@@ -3929,16 +3929,16 @@
         <v>2023</v>
       </c>
       <c r="B35" s="15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C35" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D35" s="6" t="d">
         <v>2023-10-05</v>
       </c>
       <c r="E35" s="8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F35" s="8">
         <v>8</v>
@@ -3950,19 +3950,19 @@
         <v>2023-10-07</v>
       </c>
       <c r="I35" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J35" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K35" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="L35" s="13" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="M35" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="N35" s="12">
         <v>1</v>
@@ -3977,16 +3977,16 @@
         <v>8</v>
       </c>
       <c r="R35" s="9" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="S35" s="9" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="T35" s="9" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="U35" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="V35" s="8">
         <v>0</v>
@@ -4001,40 +4001,40 @@
         <v>2023</v>
       </c>
       <c r="B36" s="15" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C36" s="8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D36" s="5" t="d">
         <v>2023-10-12</v>
       </c>
       <c r="E36" s="14" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F36" s="8">
         <v>9</v>
       </c>
       <c r="G36" s="8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H36" s="6" t="d">
         <v>2023-10-22</v>
       </c>
       <c r="I36" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J36" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K36" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="L36" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="M36" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="N36" s="12">
         <v>1</v>
@@ -4049,7 +4049,7 @@
         <v>8</v>
       </c>
       <c r="R36" s="8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="S36" s="6" t="d">
         <v>2023-11-06</v>
@@ -4076,40 +4076,40 @@
         <v>2023</v>
       </c>
       <c r="B37" s="15" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C37" s="8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D37" s="5" t="d">
         <v>2023-10-17</v>
       </c>
       <c r="E37" s="8" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F37" s="8">
         <v>6</v>
       </c>
       <c r="G37" s="8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H37" s="6" t="d">
         <v>2023-10-22</v>
       </c>
       <c r="I37" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J37" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K37" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="L37" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="M37" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="N37" s="12">
         <v>1</v>
@@ -4124,16 +4124,16 @@
         <v>7</v>
       </c>
       <c r="R37" s="9" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="S37" s="9" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="T37" s="9">
         <v>8</v>
       </c>
       <c r="U37" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="V37" s="8">
         <v>0</v>
@@ -4148,10 +4148,10 @@
         <v>2023</v>
       </c>
       <c r="B38" s="15" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C38" s="8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D38" s="5" t="d">
         <v>2023-10-20</v>
@@ -4169,19 +4169,19 @@
         <v>2023-10-22</v>
       </c>
       <c r="I38" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J38" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K38" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="L38" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="M38" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="N38" s="12">
         <v>1</v>
@@ -4202,7 +4202,7 @@
         <v>2023-11-03</v>
       </c>
       <c r="T38" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="U38" s="8">
         <v>4</v>
@@ -4233,25 +4233,25 @@
         <v>7</v>
       </c>
       <c r="G39" s="8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H39" s="6" t="d">
         <v>2024-09-06</v>
       </c>
       <c r="I39" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J39" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K39" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="L39" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="M39" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="N39" s="12">
         <v>1</v>
@@ -4284,7 +4284,7 @@
         <v>0</v>
       </c>
       <c r="X39" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="40" spans="1:37" x14ac:dyDescent="0.2">
@@ -4307,25 +4307,25 @@
         <v>9</v>
       </c>
       <c r="G40" s="8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H40" s="6" t="d">
         <v>2024-09-06</v>
       </c>
       <c r="I40" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J40" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K40" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="L40" s="13" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="M40" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="N40" s="12">
         <v>1</v>
@@ -4363,10 +4363,10 @@
         <v>2024</v>
       </c>
       <c r="B41" s="15" t="s">
+        <v>146</v>
+      </c>
+      <c r="C41" s="8" t="s">
         <v>147</v>
-      </c>
-      <c r="C41" s="8" t="s">
-        <v>148</v>
       </c>
       <c r="D41" s="4" t="d">
         <v>2024-08-24</v>
@@ -4376,25 +4376,25 @@
         <v>3</v>
       </c>
       <c r="G41" s="8" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="H41" s="6" t="d">
         <v>2024-09-06</v>
       </c>
       <c r="I41" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J41" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K41" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="L41" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="M41" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="N41" s="12">
         <v>1</v>
@@ -4415,7 +4415,7 @@
         <v>2024-09-11</v>
       </c>
       <c r="T41" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="U41" s="8">
         <v>1</v>
@@ -4447,25 +4447,25 @@
         <v>9</v>
       </c>
       <c r="G42" s="8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H42" s="6" t="d">
         <v>2024-09-27</v>
       </c>
       <c r="I42" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J42" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K42" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="L42" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="M42" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="N42" s="12">
         <v>1</v>
@@ -4518,25 +4518,25 @@
         <v>8</v>
       </c>
       <c r="G43" s="8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H43" s="6" t="d">
         <v>2024-09-27</v>
       </c>
       <c r="I43" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J43" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K43" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="L43" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="M43" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="N43" s="12">
         <v>1</v>
@@ -4574,7 +4574,7 @@
         <v>2024</v>
       </c>
       <c r="B44" s="15" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C44" s="8" t="s">
         <v>9</v>
@@ -4589,25 +4589,25 @@
         <v>5</v>
       </c>
       <c r="G44" s="8" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="H44" s="6" t="d">
         <v>2024-09-27</v>
       </c>
       <c r="I44" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J44" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K44" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="L44" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="M44" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="N44" s="12">
         <v>1</v>
@@ -4628,7 +4628,7 @@
         <v>2024-10-08</v>
       </c>
       <c r="T44" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="U44" s="8">
         <v>6</v>

</xml_diff>

<commit_message>
fixed date format of hatch begin nest BT
</commit_message>
<xml_diff>
--- a/Compiled_synchrony_experiment_data.xlsx
+++ b/Compiled_synchrony_experiment_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/justinbenjamin/Desktop/McMaster/Synchrony/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{C0F5CB93-419D-FE4D-9A7C-D0BF3E75C8A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{E245DC8E-60AD-8144-A82E-BB19ABA88C2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="13380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="411" uniqueCount="176">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="410" uniqueCount="175">
   <si>
     <t>Nest</t>
   </si>
@@ -288,9 +288,6 @@
   </si>
   <si>
     <t>NA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">05-Nov-23	</t>
   </si>
   <si>
     <t>B</t>
@@ -1472,9 +1469,9 @@
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1169386B-F813-034E-AA1A-A149472682C8}">
   <dimension ref="A1:AK145"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="W1" sqref="W1"/>
+      <selection pane="bottomLeft" activeCell="M46" sqref="M46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1514,7 +1511,7 @@
         <v>25</v>
       </c>
       <c r="F1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G1" t="s">
         <v>1</v>
@@ -1523,31 +1520,31 @@
         <v>77</v>
       </c>
       <c r="I1" t="s">
+        <v>97</v>
+      </c>
+      <c r="J1" t="s">
         <v>98</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
+        <v>134</v>
+      </c>
+      <c r="L1" t="s">
+        <v>165</v>
+      </c>
+      <c r="M1" t="s">
+        <v>96</v>
+      </c>
+      <c r="N1" t="s">
         <v>99</v>
       </c>
-      <c r="K1" t="s">
-        <v>135</v>
-      </c>
-      <c r="L1" t="s">
-        <v>166</v>
-      </c>
-      <c r="M1" t="s">
-        <v>97</v>
-      </c>
-      <c r="N1" t="s">
-        <v>100</v>
-      </c>
       <c r="O1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="P1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="Q1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="R1" t="s">
         <v>80</v>
@@ -1556,16 +1553,16 @@
         <v>81</v>
       </c>
       <c r="T1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="U1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="V1" t="s">
         <v>2</v>
       </c>
       <c r="W1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="X1" t="s">
         <v>26</v>
@@ -1576,7 +1573,7 @@
         <v>2018</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C2" s="8" t="s">
         <v>56</v>
@@ -1589,7 +1586,7 @@
         <v>7</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H2" s="6" t="d">
         <v>2018-09-03</v>
@@ -1601,13 +1598,13 @@
         <v>82</v>
       </c>
       <c r="K2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="L2" s="13" t="s">
         <v>82</v>
       </c>
       <c r="M2" s="11" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="N2" s="12">
         <v>1</v>
@@ -1640,7 +1637,7 @@
         <v>0</v>
       </c>
       <c r="X2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.2">
@@ -1648,10 +1645,10 @@
         <v>2018</v>
       </c>
       <c r="B3" s="17" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D3" s="3" t="d">
         <v>2018-08-18</v>
@@ -1661,7 +1658,7 @@
         <v>5</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="H3" s="6" t="d">
         <v>2018-09-03</v>
@@ -1679,7 +1676,7 @@
         <v>82</v>
       </c>
       <c r="M3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="N3" s="12">
         <v>1</v>
@@ -1712,7 +1709,7 @@
         <v>0</v>
       </c>
       <c r="X3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.2">
@@ -1733,7 +1730,7 @@
         <v>10</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H4" s="6" t="d">
         <v>2018-09-13</v>
@@ -1751,7 +1748,7 @@
         <v>82</v>
       </c>
       <c r="M4" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="N4" s="12">
         <v>1</v>
@@ -1784,7 +1781,7 @@
         <v>3</v>
       </c>
       <c r="X4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.2">
@@ -1805,7 +1802,7 @@
         <v>9</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H5" s="6" t="d">
         <v>2018-09-17</v>
@@ -1817,13 +1814,13 @@
         <v>82</v>
       </c>
       <c r="K5" t="s">
+        <v>141</v>
+      </c>
+      <c r="L5" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="M5" s="16" t="s">
         <v>142</v>
-      </c>
-      <c r="L5" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="M5" s="16" t="s">
-        <v>143</v>
       </c>
       <c r="N5" s="8">
         <v>2</v>
@@ -1856,7 +1853,7 @@
         <v>2</v>
       </c>
       <c r="X5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.2">
@@ -1864,10 +1861,10 @@
         <v>2018</v>
       </c>
       <c r="B6" s="17" t="s">
+        <v>155</v>
+      </c>
+      <c r="C6" s="8" t="s">
         <v>156</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>157</v>
       </c>
       <c r="D6" s="3" t="d">
         <v>2018-09-15</v>
@@ -1877,7 +1874,7 @@
         <v>9</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H6" s="6" t="d">
         <v>2018-09-17</v>
@@ -1895,7 +1892,7 @@
         <v>82</v>
       </c>
       <c r="M6" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="N6" s="12">
         <v>1</v>
@@ -1946,7 +1943,7 @@
         <v>7</v>
       </c>
       <c r="G7" s="8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H7" s="6" t="d">
         <v>2018-09-17</v>
@@ -1964,7 +1961,7 @@
         <v>82</v>
       </c>
       <c r="M7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="N7" s="12">
         <v>1</v>
@@ -1997,7 +1994,7 @@
         <v>3</v>
       </c>
       <c r="X7" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.2">
@@ -2005,10 +2002,10 @@
         <v>2018</v>
       </c>
       <c r="B8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D8" s="3" t="d">
         <v>2018-09-12</v>
@@ -2018,7 +2015,7 @@
         <v>5</v>
       </c>
       <c r="G8" s="8" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="H8" s="6" t="d">
         <v>2018-09-17</v>
@@ -2036,7 +2033,7 @@
         <v>82</v>
       </c>
       <c r="M8" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="N8" s="12">
         <v>1</v>
@@ -2087,7 +2084,7 @@
         <v>7</v>
       </c>
       <c r="G9" s="8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H9" s="6" t="d">
         <v>2018-09-01</v>
@@ -2105,7 +2102,7 @@
         <v>82</v>
       </c>
       <c r="M9" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="N9" s="12">
         <v>1</v>
@@ -2156,7 +2153,7 @@
         <v>5</v>
       </c>
       <c r="G10" s="8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H10" s="6" t="d">
         <v>2018-09-01</v>
@@ -2174,7 +2171,7 @@
         <v>82</v>
       </c>
       <c r="M10" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="N10" s="12">
         <v>1</v>
@@ -2207,7 +2204,7 @@
         <v>3</v>
       </c>
       <c r="X10" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="11" spans="1:24" x14ac:dyDescent="0.2">
@@ -2228,7 +2225,7 @@
         <v>7</v>
       </c>
       <c r="G11" s="8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H11" s="6" t="d">
         <v>2018-08-30</v>
@@ -2240,13 +2237,13 @@
         <v>82</v>
       </c>
       <c r="K11" s="15" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="L11" s="8" t="s">
         <v>82</v>
       </c>
       <c r="M11" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="N11" s="8">
         <v>2</v>
@@ -2279,7 +2276,7 @@
         <v>2</v>
       </c>
       <c r="X11" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="12" spans="1:24" x14ac:dyDescent="0.2">
@@ -2300,7 +2297,7 @@
         <v>8</v>
       </c>
       <c r="G12" s="8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H12" s="6" t="d">
         <v>2018-08-28</v>
@@ -2318,7 +2315,7 @@
         <v>82</v>
       </c>
       <c r="M12" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="N12" s="12">
         <v>1</v>
@@ -2351,7 +2348,7 @@
         <v>2</v>
       </c>
       <c r="X12" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="13" spans="1:24" x14ac:dyDescent="0.2">
@@ -2372,7 +2369,7 @@
         <v>10</v>
       </c>
       <c r="G13" s="8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H13" s="6" t="d">
         <v>2018-09-13</v>
@@ -2384,13 +2381,13 @@
         <v>82</v>
       </c>
       <c r="K13" t="s">
+        <v>138</v>
+      </c>
+      <c r="L13" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="M13" t="s">
         <v>139</v>
-      </c>
-      <c r="L13" s="13" t="s">
-        <v>82</v>
-      </c>
-      <c r="M13" t="s">
-        <v>140</v>
       </c>
       <c r="N13" s="8">
         <v>2</v>
@@ -2441,7 +2438,7 @@
         <v>8</v>
       </c>
       <c r="G14" s="8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H14" s="6" t="d">
         <v>2018-09-17</v>
@@ -2459,7 +2456,7 @@
         <v>82</v>
       </c>
       <c r="M14" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="N14" s="12">
         <v>1</v>
@@ -2510,7 +2507,7 @@
         <v>8</v>
       </c>
       <c r="G15" s="8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H15" s="6" t="d">
         <v>2018-09-17</v>
@@ -2528,7 +2525,7 @@
         <v>82</v>
       </c>
       <c r="M15" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="N15" s="12">
         <v>1</v>
@@ -2566,7 +2563,7 @@
         <v>2018</v>
       </c>
       <c r="B16" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C16" s="8" t="s">
         <v>67</v>
@@ -2579,7 +2576,7 @@
         <v>6</v>
       </c>
       <c r="G16" s="8" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="H16" s="6" t="d">
         <v>2018-09-22</v>
@@ -2591,13 +2588,13 @@
         <v>82</v>
       </c>
       <c r="K16" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="L16" s="8" t="s">
         <v>82</v>
       </c>
       <c r="M16" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="N16" s="12">
         <v>2</v>
@@ -2646,7 +2643,7 @@
         <v>7</v>
       </c>
       <c r="G17" s="8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H17" s="6" t="d">
         <v>2018-09-22</v>
@@ -2658,13 +2655,13 @@
         <v>82</v>
       </c>
       <c r="K17" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="L17" s="8" t="s">
         <v>82</v>
       </c>
       <c r="M17" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="N17" s="8">
         <v>2</v>
@@ -2715,7 +2712,7 @@
         <v>12</v>
       </c>
       <c r="G18" s="8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H18" s="6" t="d">
         <v>2018-09-27</v>
@@ -2733,7 +2730,7 @@
         <v>82</v>
       </c>
       <c r="M18" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="N18" s="12">
         <v>1</v>
@@ -2766,7 +2763,7 @@
         <v>0</v>
       </c>
       <c r="X18" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="19" spans="1:34" x14ac:dyDescent="0.2">
@@ -2787,7 +2784,7 @@
         <v>6</v>
       </c>
       <c r="G19" s="8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H19" s="6" t="d">
         <v>2018-09-15</v>
@@ -2799,13 +2796,13 @@
         <v>82</v>
       </c>
       <c r="K19" s="15" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="L19" s="8" t="s">
         <v>82</v>
       </c>
       <c r="M19" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="N19" s="8">
         <v>2</v>
@@ -2856,7 +2853,7 @@
         <v>7</v>
       </c>
       <c r="G20" s="8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H20" s="6" t="d">
         <v>2018-09-22</v>
@@ -2874,7 +2871,7 @@
         <v>82</v>
       </c>
       <c r="M20" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="N20" s="8">
         <v>1</v>
@@ -2925,7 +2922,7 @@
         <v>7</v>
       </c>
       <c r="G21" s="8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H21" s="6" t="d">
         <v>2018-09-19</v>
@@ -2937,13 +2934,13 @@
         <v>2018-09-30</v>
       </c>
       <c r="K21" t="s">
+        <v>168</v>
+      </c>
+      <c r="L21" t="s">
         <v>169</v>
       </c>
-      <c r="L21" t="s">
-        <v>170</v>
-      </c>
       <c r="M21" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="N21" s="12">
         <v>3</v>
@@ -2994,7 +2991,7 @@
         <v>8</v>
       </c>
       <c r="G22" s="8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H22" s="8" t="s">
         <v>82</v>
@@ -3012,7 +3009,7 @@
         <v>82</v>
       </c>
       <c r="M22" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="N22" s="12">
         <v>0</v>
@@ -3045,7 +3042,7 @@
         <v>3</v>
       </c>
       <c r="X22" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="Z22" s="8"/>
     </row>
@@ -3067,7 +3064,7 @@
         <v>6</v>
       </c>
       <c r="G23" s="8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H23" s="8" t="s">
         <v>82</v>
@@ -3085,7 +3082,7 @@
         <v>82</v>
       </c>
       <c r="M23" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="N23" s="12">
         <v>0</v>
@@ -3118,7 +3115,7 @@
         <v>4</v>
       </c>
       <c r="X23" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="Z23" s="8"/>
     </row>
@@ -3140,7 +3137,7 @@
         <v>7</v>
       </c>
       <c r="G24" s="8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H24" s="8" t="s">
         <v>82</v>
@@ -3158,7 +3155,7 @@
         <v>82</v>
       </c>
       <c r="M24" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="N24" s="8">
         <v>0</v>
@@ -3191,7 +3188,7 @@
         <v>3</v>
       </c>
       <c r="X24" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="Z24" s="8"/>
     </row>
@@ -3213,7 +3210,7 @@
         <v>7</v>
       </c>
       <c r="G25" s="8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H25" s="8" t="s">
         <v>82</v>
@@ -3231,7 +3228,7 @@
         <v>82</v>
       </c>
       <c r="M25" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="N25" s="12">
         <v>0</v>
@@ -3264,7 +3261,7 @@
         <v>2</v>
       </c>
       <c r="X25" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="Z25" s="8"/>
     </row>
@@ -3288,7 +3285,7 @@
         <v>8</v>
       </c>
       <c r="G26" s="8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H26" s="6" t="d">
         <v>2023-09-04</v>
@@ -3306,7 +3303,7 @@
         <v>82</v>
       </c>
       <c r="M26" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="N26" s="12">
         <v>1</v>
@@ -3362,7 +3359,7 @@
         <v>8</v>
       </c>
       <c r="G27" s="8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H27" s="6" t="d">
         <v>2023-09-04</v>
@@ -3380,7 +3377,7 @@
         <v>82</v>
       </c>
       <c r="M27" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="N27" s="12">
         <v>1</v>
@@ -3421,10 +3418,10 @@
         <v>2023</v>
       </c>
       <c r="B28" s="15" t="s">
+        <v>149</v>
+      </c>
+      <c r="C28" s="8" t="s">
         <v>150</v>
-      </c>
-      <c r="C28" s="8" t="s">
-        <v>151</v>
       </c>
       <c r="D28" s="5" t="d">
         <v>2023-08-20</v>
@@ -3434,7 +3431,7 @@
         <v>5</v>
       </c>
       <c r="G28" s="8" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="H28" s="6" t="d">
         <v>2023-09-04</v>
@@ -3452,7 +3449,7 @@
         <v>82</v>
       </c>
       <c r="M28" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="N28" s="12">
         <v>1</v>
@@ -3526,7 +3523,7 @@
         <v>82</v>
       </c>
       <c r="M29" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="N29" s="12">
         <v>1</v>
@@ -3581,7 +3578,7 @@
         <v>12</v>
       </c>
       <c r="G30" s="8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H30" s="6" t="d">
         <v>2023-09-15</v>
@@ -3599,7 +3596,7 @@
         <v>82</v>
       </c>
       <c r="M30" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="N30" s="12">
         <v>1</v>
@@ -3654,7 +3651,7 @@
         <v>9</v>
       </c>
       <c r="G31" s="8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H31" s="6" t="d">
         <v>2023-09-15</v>
@@ -3672,7 +3669,7 @@
         <v>82</v>
       </c>
       <c r="M31" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="N31" s="12">
         <v>1</v>
@@ -3745,7 +3742,7 @@
         <v>82</v>
       </c>
       <c r="M32" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="N32" s="12">
         <v>1</v>
@@ -3800,7 +3797,7 @@
         <v>8</v>
       </c>
       <c r="G33" s="8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H33" s="6" t="d">
         <v>2023-10-07</v>
@@ -3818,7 +3815,7 @@
         <v>82</v>
       </c>
       <c r="M33" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="N33" s="12">
         <v>1</v>
@@ -3872,7 +3869,7 @@
         <v>8</v>
       </c>
       <c r="G34" s="8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H34" s="6" t="d">
         <v>2023-10-07</v>
@@ -3890,7 +3887,7 @@
         <v>82</v>
       </c>
       <c r="M34" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="N34" s="12">
         <v>1</v>
@@ -3962,7 +3959,7 @@
         <v>82</v>
       </c>
       <c r="M35" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="N35" s="12">
         <v>1</v>
@@ -4016,7 +4013,7 @@
         <v>9</v>
       </c>
       <c r="G36" s="8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H36" s="6" t="d">
         <v>2023-10-22</v>
@@ -4034,7 +4031,7 @@
         <v>82</v>
       </c>
       <c r="M36" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="N36" s="12">
         <v>1</v>
@@ -4048,8 +4045,8 @@
       <c r="Q36" s="8">
         <v>8</v>
       </c>
-      <c r="R36" s="8" t="s">
-        <v>83</v>
+      <c r="R36" s="6" t="d">
+        <v>2023-11-05</v>
       </c>
       <c r="S36" s="6" t="d">
         <v>2023-11-06</v>
@@ -4085,13 +4082,13 @@
         <v>2023-10-17</v>
       </c>
       <c r="E37" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F37" s="8">
         <v>6</v>
       </c>
       <c r="G37" s="8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H37" s="6" t="d">
         <v>2023-10-22</v>
@@ -4109,7 +4106,7 @@
         <v>82</v>
       </c>
       <c r="M37" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="N37" s="12">
         <v>1</v>
@@ -4181,7 +4178,7 @@
         <v>82</v>
       </c>
       <c r="M38" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="N38" s="12">
         <v>1</v>
@@ -4233,7 +4230,7 @@
         <v>7</v>
       </c>
       <c r="G39" s="8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H39" s="6" t="d">
         <v>2024-09-06</v>
@@ -4251,7 +4248,7 @@
         <v>82</v>
       </c>
       <c r="M39" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="N39" s="12">
         <v>1</v>
@@ -4307,7 +4304,7 @@
         <v>9</v>
       </c>
       <c r="G40" s="8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H40" s="6" t="d">
         <v>2024-09-06</v>
@@ -4325,7 +4322,7 @@
         <v>82</v>
       </c>
       <c r="M40" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="N40" s="12">
         <v>1</v>
@@ -4363,10 +4360,10 @@
         <v>2024</v>
       </c>
       <c r="B41" s="15" t="s">
+        <v>145</v>
+      </c>
+      <c r="C41" s="8" t="s">
         <v>146</v>
-      </c>
-      <c r="C41" s="8" t="s">
-        <v>147</v>
       </c>
       <c r="D41" s="4" t="d">
         <v>2024-08-24</v>
@@ -4376,7 +4373,7 @@
         <v>3</v>
       </c>
       <c r="G41" s="8" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="H41" s="6" t="d">
         <v>2024-09-06</v>
@@ -4394,7 +4391,7 @@
         <v>82</v>
       </c>
       <c r="M41" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="N41" s="12">
         <v>1</v>
@@ -4447,7 +4444,7 @@
         <v>9</v>
       </c>
       <c r="G42" s="8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H42" s="6" t="d">
         <v>2024-09-27</v>
@@ -4465,7 +4462,7 @@
         <v>82</v>
       </c>
       <c r="M42" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="N42" s="12">
         <v>1</v>
@@ -4518,7 +4515,7 @@
         <v>8</v>
       </c>
       <c r="G43" s="8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H43" s="6" t="d">
         <v>2024-09-27</v>
@@ -4536,7 +4533,7 @@
         <v>82</v>
       </c>
       <c r="M43" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="N43" s="12">
         <v>1</v>
@@ -4574,7 +4571,7 @@
         <v>2024</v>
       </c>
       <c r="B44" s="15" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C44" s="8" t="s">
         <v>9</v>
@@ -4589,7 +4586,7 @@
         <v>5</v>
       </c>
       <c r="G44" s="8" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="H44" s="6" t="d">
         <v>2024-09-27</v>
@@ -4607,7 +4604,7 @@
         <v>82</v>
       </c>
       <c r="M44" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="N44" s="12">
         <v>1</v>

</xml_diff>